<commit_message>
Revisi 2 erd dan excel
</commit_message>
<xml_diff>
--- a/Normalisasi.xlsx
+++ b/Normalisasi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frederick\Documents\Kuliah\OOP\TugasAkhir_Restaurant_OOP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9DE6BE-DA77-45E8-8045-841EDA7AFA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DABBBF-31D4-4DCA-9D3A-F76083F1E383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{BAA0767E-DF80-4FFD-B866-E03C755585BA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{BAA0767E-DF80-4FFD-B866-E03C755585BA}"/>
   </bookViews>
   <sheets>
     <sheet name="UNF" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="107">
   <si>
     <t>Table Type</t>
   </si>
@@ -275,9 +275,6 @@
     <t>AvailableOn</t>
   </si>
   <si>
-    <t>Restaurant +B2:R2Invoice</t>
-  </si>
-  <si>
     <t>MenuID (PK)</t>
   </si>
   <si>
@@ -345,6 +342,24 @@
   </si>
   <si>
     <t>LocationID (PK)</t>
+  </si>
+  <si>
+    <t>Restaurant Invoice</t>
+  </si>
+  <si>
+    <t>Reserved Time</t>
+  </si>
+  <si>
+    <t>12 Jan 2020,11:00</t>
+  </si>
+  <si>
+    <t>13 Jan 2020,11:00</t>
+  </si>
+  <si>
+    <t>15 Jan 2020,11:00</t>
+  </si>
+  <si>
+    <t>20 Jan 2020,11:00</t>
   </si>
 </sst>
 </file>
@@ -400,7 +415,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -443,48 +458,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -510,22 +488,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -537,13 +500,16 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -880,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2319B30-2675-4DDB-92EA-94A7A14FC08F}">
-  <dimension ref="B2:R11"/>
+  <dimension ref="B2:S11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:D12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -892,26 +858,27 @@
     <col min="2" max="2" width="7.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.08984375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="174.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.7265625" style="2"/>
+    <col min="5" max="5" width="15.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="174.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B2" s="13" t="s">
-        <v>78</v>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B2" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -929,8 +896,9 @@
       <c r="P2" s="14"/>
       <c r="Q2" s="14"/>
       <c r="R2" s="14"/>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S2" s="14"/>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>52</v>
       </c>
@@ -941,49 +909,52 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="H3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="R3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>53</v>
       </c>
@@ -993,170 +964,178 @@
       <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="3">
-        <v>2</v>
-      </c>
       <c r="H4" s="3">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3">
         <v>1</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="3">
-        <v>2</v>
-      </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="3">
+        <v>2</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="3">
+      <c r="O4" s="3">
         <v>1</v>
       </c>
-      <c r="O4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="R4" s="5">
         <v>1000000</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B5" s="12" t="s">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="3">
-        <v>4</v>
-      </c>
       <c r="H5" s="3">
+        <v>4</v>
+      </c>
+      <c r="I5" s="3">
         <v>1</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="3">
-        <v>4</v>
-      </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="3">
+        <v>4</v>
+      </c>
+      <c r="L5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="18" t="s">
+      <c r="N5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="3">
-        <v>2</v>
-      </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="3">
+        <v>2</v>
+      </c>
+      <c r="P5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="Q5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="R5" s="5">
         <v>250000</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="S5" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="9" t="s">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="9">
+      <c r="H6" s="9">
         <v>10</v>
       </c>
-      <c r="H6" s="9">
+      <c r="I6" s="9">
         <v>1</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="12">
+      <c r="J6" s="9"/>
+      <c r="K6" s="9">
         <v>8</v>
       </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="9"/>
+      <c r="M6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="19"/>
-      <c r="N6" s="3">
-        <v>4</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>18</v>
+      <c r="N6" s="16"/>
+      <c r="O6" s="3">
+        <v>4</v>
       </c>
       <c r="P6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="Q6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R6" s="5">
         <v>100000</v>
       </c>
-      <c r="R6" s="10"/>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="3" t="s">
+      <c r="S6" s="9"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M7" s="20"/>
-      <c r="N7" s="3">
+      <c r="N7" s="16"/>
+      <c r="O7" s="3">
         <v>3</v>
       </c>
-      <c r="O7" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="P7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="Q7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R7" s="5">
         <v>80000</v>
       </c>
-      <c r="R7" s="11"/>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B8" s="12" t="s">
+      <c r="S7" s="9"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B8" s="9" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -1166,79 +1145,83 @@
         <v>36</v>
       </c>
       <c r="E8" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="9">
+      <c r="H8" s="9">
         <v>10</v>
       </c>
-      <c r="H8" s="9">
-        <v>2</v>
-      </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="9">
+        <v>2</v>
+      </c>
+      <c r="J8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="9">
+      <c r="K8" s="9">
         <v>17</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="L8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M8" s="18" t="s">
+      <c r="N8" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="N8" s="3">
-        <v>4</v>
-      </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="3">
+        <v>4</v>
+      </c>
+      <c r="P8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="Q8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="R8" s="5">
         <v>100000</v>
       </c>
-      <c r="R8" s="9" t="s">
+      <c r="S8" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B9" s="12"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="3" t="s">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="M9" s="20"/>
-      <c r="N9" s="3">
+      <c r="N9" s="16"/>
+      <c r="O9" s="3">
         <v>28</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="P9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="Q9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="R9" s="5">
         <v>20000</v>
       </c>
-      <c r="R9" s="11"/>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B10" s="12" t="s">
+      <c r="S9" s="9"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B10" s="9" t="s">
         <v>56</v>
       </c>
       <c r="C10" s="9" t="s">
@@ -1248,120 +1231,127 @@
         <v>47</v>
       </c>
       <c r="E10" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="3">
-        <v>2</v>
-      </c>
       <c r="H10" s="3">
         <v>2</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="3">
+        <v>2</v>
+      </c>
+      <c r="J10" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="3">
-        <v>4</v>
-      </c>
-      <c r="K10" s="9" t="s">
+      <c r="K10" s="3">
+        <v>4</v>
+      </c>
+      <c r="L10" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M10" s="18" t="s">
+      <c r="N10" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="N10" s="3">
-        <v>2</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>18</v>
+      <c r="O10" s="3">
+        <v>2</v>
       </c>
       <c r="P10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="Q10" s="5">
+      <c r="Q10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R10" s="5">
         <v>30000</v>
       </c>
-      <c r="R10" s="9" t="s">
+      <c r="S10" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B11" s="12"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="3" t="s">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="3">
-        <v>4</v>
-      </c>
       <c r="H11" s="3">
+        <v>4</v>
+      </c>
+      <c r="I11" s="3">
         <v>1</v>
       </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="3">
-        <v>4</v>
-      </c>
-      <c r="K11" s="11"/>
-      <c r="L11" s="3" t="s">
+      <c r="J11" s="9"/>
+      <c r="K11" s="3">
+        <v>4</v>
+      </c>
+      <c r="L11" s="9"/>
+      <c r="M11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="M11" s="20"/>
-      <c r="N11" s="3">
-        <v>4</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>18</v>
+      <c r="N11" s="16"/>
+      <c r="O11" s="3">
+        <v>4</v>
       </c>
       <c r="P11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="Q11" s="5">
+      <c r="Q11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R11" s="5">
         <v>35000</v>
       </c>
-      <c r="R11" s="11"/>
+      <c r="S11" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="R10:R11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="B2:R2"/>
-    <mergeCell ref="J6:J7"/>
+  <mergeCells count="36">
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="S5:S7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="N5:N7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="K6:K7"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="J8:J9"/>
     <mergeCell ref="K8:K9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S8:S9"/>
     <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="K5:K7"/>
-    <mergeCell ref="R5:R7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="M5:M7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="L5:L7"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="S10:S11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1370,59 +1360,61 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C07B70A-99B4-47B8-881F-63A149D8C03F}">
-  <dimension ref="B2:S11"/>
+  <dimension ref="B2:T11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4:N11"/>
+      <selection activeCell="E3" sqref="E3:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="2"/>
-    <col min="2" max="2" width="15.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="175.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.7265625" style="2"/>
+    <col min="2" max="2" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.36328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="180.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B2" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-    </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>57</v>
       </c>
@@ -1433,52 +1425,55 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="H3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="R3" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="S3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>53</v>
       </c>
@@ -1488,53 +1483,56 @@
       <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="3">
-        <v>2</v>
-      </c>
       <c r="H4" s="3">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3">
         <v>1</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="3">
-        <v>2</v>
-      </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="3">
+        <v>2</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="3">
+      <c r="P4" s="3">
         <v>1</v>
       </c>
-      <c r="P4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q4" s="3" t="s">
+      <c r="Q4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="R4" s="5">
+      <c r="S4" s="5">
         <v>1000000</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>54</v>
       </c>
@@ -1544,53 +1542,56 @@
       <c r="D5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="3">
-        <v>4</v>
-      </c>
       <c r="H5" s="3">
+        <v>4</v>
+      </c>
+      <c r="I5" s="3">
         <v>1</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="3">
-        <v>4</v>
-      </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="3">
+        <v>4</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="O5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="O5" s="3">
-        <v>2</v>
-      </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="R5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="R5" s="5">
+      <c r="S5" s="5">
         <v>250000</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="T5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>54</v>
       </c>
@@ -1600,53 +1601,56 @@
       <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <v>10</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <v>1</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="3">
+      <c r="K6" s="3">
         <v>8</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="O6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="3">
-        <v>4</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>18</v>
+      <c r="P6" s="3">
+        <v>4</v>
       </c>
       <c r="Q6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="S6" s="5">
         <v>100000</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="T6" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
         <v>54</v>
       </c>
@@ -1656,53 +1660,56 @@
       <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>10</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="3">
         <v>1</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="3">
+      <c r="K7" s="3">
         <v>8</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="O7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="O7" s="3">
+      <c r="P7" s="3">
         <v>3</v>
       </c>
-      <c r="P7" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="Q7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="R7" s="5">
+      <c r="R7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="S7" s="5">
         <v>80000</v>
       </c>
-      <c r="S7" s="3" t="s">
+      <c r="T7" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>55</v>
       </c>
@@ -1713,52 +1720,55 @@
         <v>36</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <v>10</v>
       </c>
-      <c r="H8" s="3">
-        <v>2</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="3">
+        <v>2</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="3">
+      <c r="K8" s="3">
         <v>17</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="8" t="s">
+      <c r="O8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="O8" s="3">
-        <v>4</v>
-      </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="R8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="R8" s="5">
+      <c r="S8" s="5">
         <v>100000</v>
       </c>
-      <c r="S8" s="3" t="s">
+      <c r="T8" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
         <v>55</v>
       </c>
@@ -1769,52 +1779,55 @@
         <v>36</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>10</v>
       </c>
-      <c r="H9" s="3">
-        <v>2</v>
-      </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="3">
+        <v>2</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="3">
+      <c r="K9" s="3">
         <v>17</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N9" s="8" t="s">
+      <c r="O9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="O9" s="3">
+      <c r="P9" s="3">
         <v>28</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="Q9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="Q9" s="3" t="s">
+      <c r="R9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="R9" s="5">
+      <c r="S9" s="5">
         <v>20000</v>
       </c>
-      <c r="S9" s="3" t="s">
+      <c r="T9" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>56</v>
       </c>
@@ -1825,52 +1838,55 @@
         <v>47</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="3">
-        <v>2</v>
-      </c>
       <c r="H10" s="3">
         <v>2</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="3">
+        <v>2</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="3">
-        <v>4</v>
-      </c>
-      <c r="K10" s="3" t="s">
+      <c r="K10" s="3">
+        <v>4</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="N10" s="8" t="s">
+      <c r="O10" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="O10" s="3">
-        <v>2</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>18</v>
+      <c r="P10" s="3">
+        <v>2</v>
       </c>
       <c r="Q10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="R10" s="5">
+      <c r="R10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="S10" s="5">
         <v>30000</v>
       </c>
-      <c r="S10" s="3" t="s">
+      <c r="T10" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
         <v>56</v>
       </c>
@@ -1881,54 +1897,57 @@
         <v>47</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="3">
-        <v>4</v>
-      </c>
       <c r="H11" s="3">
+        <v>4</v>
+      </c>
+      <c r="I11" s="3">
         <v>1</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="J11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="3">
-        <v>4</v>
-      </c>
-      <c r="K11" s="3" t="s">
+      <c r="K11" s="3">
+        <v>4</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="N11" s="8" t="s">
+      <c r="O11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="O11" s="3">
-        <v>4</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>18</v>
+      <c r="P11" s="3">
+        <v>4</v>
       </c>
       <c r="Q11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="R11" s="5">
+      <c r="R11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="S11" s="5">
         <v>35000</v>
       </c>
-      <c r="S11" s="3" t="s">
+      <c r="T11" s="3" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="B2:T2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1937,28 +1956,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D07283-676B-4F48-9B92-322057909C13}">
-  <dimension ref="B2:N22"/>
+  <dimension ref="B2:O22"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+      <selection activeCell="C14" sqref="C14:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="2"/>
-    <col min="2" max="3" width="14.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="174.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="174.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="175.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.26953125" style="2" bestFit="1" customWidth="1"/>
@@ -1966,19 +1986,19 @@
     <col min="20" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B2" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>57</v>
       </c>
@@ -1992,7 +2012,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>8</v>
@@ -2004,7 +2024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
         <v>53</v>
       </c>
@@ -2029,11 +2049,8 @@
       <c r="I4" s="8">
         <v>2</v>
       </c>
-      <c r="N4" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>54</v>
       </c>
@@ -2058,11 +2075,8 @@
       <c r="I5" s="8">
         <v>4</v>
       </c>
-      <c r="N5" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>54</v>
       </c>
@@ -2087,11 +2101,8 @@
       <c r="I6" s="8">
         <v>8</v>
       </c>
-      <c r="N6" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>54</v>
       </c>
@@ -2116,11 +2127,8 @@
       <c r="I7" s="8">
         <v>8</v>
       </c>
-      <c r="N7" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B8" s="8" t="s">
         <v>55</v>
       </c>
@@ -2145,11 +2153,8 @@
       <c r="I8" s="8">
         <v>17</v>
       </c>
-      <c r="N8" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B9" s="8" t="s">
         <v>55</v>
       </c>
@@ -2174,11 +2179,8 @@
       <c r="I9" s="8">
         <v>17</v>
       </c>
-      <c r="N9" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B10" s="8" t="s">
         <v>56</v>
       </c>
@@ -2203,11 +2205,8 @@
       <c r="I10" s="8">
         <v>4</v>
       </c>
-      <c r="N10" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B11" s="8" t="s">
         <v>56</v>
       </c>
@@ -2232,303 +2231,316 @@
       <c r="I11" s="8">
         <v>4</v>
       </c>
-      <c r="N11" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="16" t="s">
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B13" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="I13" s="16" t="s">
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="J13" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
         <v>70</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="F14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="O14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B15" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="E15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="F15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="G15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="J15" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="K15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="L15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M15" s="3" t="s">
+      <c r="M15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="N15" s="5">
+      <c r="O15" s="5">
         <v>1000000</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="E16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="F16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="G16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="J16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="K16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="L16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="N16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="N16" s="5">
+      <c r="O16" s="5">
         <v>250000</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B17" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="F17" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="G17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="J17" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="K17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="8" t="s">
+      <c r="L17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="M17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N17" s="5">
+      <c r="N17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O17" s="5">
         <v>100000</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B18" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="F18" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="G18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="J18" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="K18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="L18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="M18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N18" s="5">
+      <c r="N18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O18" s="5">
         <v>80000</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="I19" s="8" t="s">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="J19" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="K19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="L19" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="M19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="M19" s="3" t="s">
+      <c r="N19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="N19" s="5">
+      <c r="O19" s="5">
         <v>100000</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="I20" s="8" t="s">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="J20" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="K20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="L20" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="M20" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="M20" s="3" t="s">
+      <c r="N20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="N20" s="5">
+      <c r="O20" s="5">
         <v>20000</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="I21" s="8" t="s">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="J21" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="K21" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="L21" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="L21" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="M21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N21" s="5">
+      <c r="N21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O21" s="5">
         <v>30000</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="I22" s="8" t="s">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="J22" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="K22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K22" s="8" t="s">
+      <c r="L22" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="L22" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="M22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N22" s="5">
+      <c r="N22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O22" s="5">
         <v>35000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="I13:N13"/>
+    <mergeCell ref="J13:O13"/>
     <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B13:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2538,8 +2550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF8BA7B-1052-4466-9279-73517970B9C2}">
   <dimension ref="B2:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15:H22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2547,8 +2559,7 @@
     <col min="1" max="1" width="8.7265625" style="2"/>
     <col min="2" max="2" width="15" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.90625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.36328125" style="2" bestFit="1" customWidth="1"/>
@@ -2566,18 +2577,18 @@
     <col min="20" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B2" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>57</v>
       </c>
@@ -2588,7 +2599,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -2600,7 +2611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
         <v>53</v>
       </c>
@@ -2611,7 +2622,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4" s="8">
         <v>1</v>
@@ -2623,7 +2634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>54</v>
       </c>
@@ -2634,7 +2645,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F5" s="8">
         <v>1</v>
@@ -2646,7 +2657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>54</v>
       </c>
@@ -2657,7 +2668,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F6" s="8">
         <v>1</v>
@@ -2669,7 +2680,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>54</v>
       </c>
@@ -2680,7 +2691,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F7" s="8">
         <v>1</v>
@@ -2692,7 +2703,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B8" s="8" t="s">
         <v>55</v>
       </c>
@@ -2703,7 +2714,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F8" s="8">
         <v>2</v>
@@ -2715,7 +2726,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9" s="8" t="s">
         <v>55</v>
       </c>
@@ -2726,7 +2737,7 @@
         <v>28</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F9" s="8">
         <v>2</v>
@@ -2738,7 +2749,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="8" t="s">
         <v>56</v>
       </c>
@@ -2749,7 +2760,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F10" s="8">
         <v>2</v>
@@ -2761,7 +2772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" s="8" t="s">
         <v>56</v>
       </c>
@@ -2772,7 +2783,7 @@
         <v>4</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F11" s="8">
         <v>1</v>
@@ -2784,105 +2795,115 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B13" s="16" t="s">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B13" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="F13" s="16" t="s">
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="G13" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B15" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="G15" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="I15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="3" t="s">
+      <c r="J15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K15" s="5">
+      <c r="L15" s="5">
         <v>1000000</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="G16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="I16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="K16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K16" s="5">
+      <c r="L16" s="5">
         <v>250000</v>
       </c>
     </row>
@@ -2891,27 +2912,30 @@
         <v>55</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="G17" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="I17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I17" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="J17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K17" s="5">
+      <c r="K17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" s="5">
         <v>100000</v>
       </c>
     </row>
@@ -2920,107 +2944,110 @@
         <v>56</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="G18" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="I18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="J18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K18" s="5">
+      <c r="K18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" s="5">
         <v>80000</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="F19" s="8" t="s">
+      <c r="G19" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="I19" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="J19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="K19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="K19" s="5">
+      <c r="L19" s="5">
         <v>100000</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B20" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="F20" s="8" t="s">
+      <c r="B20" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="G20" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="I20" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="J20" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="K20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="K20" s="5">
+      <c r="L20" s="5">
         <v>20000</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F21" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="H21" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="I21" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="I21" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="J21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K21" s="5">
+      <c r="K21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L21" s="5">
         <v>30000</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>15</v>
@@ -3028,28 +3055,28 @@
       <c r="D22" s="8">
         <v>2</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="G22" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="I22" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="I22" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="J22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K22" s="5">
+      <c r="K22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L22" s="5">
         <v>35000</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B23" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>24</v>
@@ -3060,7 +3087,7 @@
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>25</v>
@@ -3070,43 +3097,43 @@
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="F26" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="J26" s="17" t="s">
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="F26" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="J26" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>2</v>
@@ -3123,19 +3150,19 @@
         <v>16</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K28" s="8" t="s">
         <v>14</v>
@@ -3152,19 +3179,19 @@
         <v>29</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>20</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>21</v>
@@ -3181,19 +3208,19 @@
         <v>39</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K30" s="8" t="s">
         <v>36</v>
@@ -3210,19 +3237,19 @@
         <v>49</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>46</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K31" s="8" t="s">
         <v>47</v>
@@ -3235,11 +3262,11 @@
   <mergeCells count="7">
     <mergeCell ref="J26:L26"/>
     <mergeCell ref="B2:H2"/>
-    <mergeCell ref="F13:K13"/>
+    <mergeCell ref="G13:L13"/>
     <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B13:D13"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B13:E13"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>